<commit_message>
added 19 n 26 articles
</commit_message>
<xml_diff>
--- a/locales.xlsx
+++ b/locales.xlsx
@@ -164,9 +164,6 @@
     <t>EN</t>
   </si>
   <si>
-    <t>VN</t>
-  </si>
-  <si>
     <t>ARTICLES</t>
   </si>
   <si>
@@ -319,6 +316,10 @@
   </si>
   <si>
     <t>Vô tình hủy đăng ký? Đăng ký lại</t>
+  </si>
+  <si>
+    <t>VI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -691,7 +692,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:Y9"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -708,7 +709,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -719,7 +720,7 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
@@ -736,7 +737,7 @@
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -748,29 +749,29 @@
         <v>6</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -787,7 +788,7 @@
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -799,12 +800,12 @@
         <v>15</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>16</v>
@@ -816,12 +817,12 @@
         <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>19</v>
@@ -833,12 +834,12 @@
         <v>21</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>22</v>
@@ -847,10 +848,10 @@
         <v>23</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -875,7 +876,7 @@
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>24</v>
@@ -887,12 +888,12 @@
         <v>26</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>27</v>
@@ -904,12 +905,12 @@
         <v>29</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>30</v>
@@ -921,12 +922,12 @@
         <v>32</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>33</v>
@@ -943,7 +944,7 @@
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>37</v>
@@ -952,13 +953,13 @@
         <v>38</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>39</v>
@@ -967,22 +968,22 @@
         <v>40</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" s="7"/>
     </row>
@@ -995,78 +996,78 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="7"/>

</xml_diff>